<commit_message>
Interim commit before resumption of converting Excel to .rda files on 2 May 2016
</commit_message>
<xml_diff>
--- a/data-raw/ITNS-Ch08-Excercises data - paired-gdc.xlsx
+++ b/data-raw/ITNS-Ch08-Excercises data - paired-gdc.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17115" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17115" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Emotion_HeartRate Ex 3" sheetId="11" r:id="rId1"/>
-    <sheet name="labels_and_flavor Ex 4" sheetId="7" r:id="rId2"/>
+    <sheet name="emotion_heartrate" sheetId="11" r:id="rId1"/>
+    <sheet name="labels_flavor" sheetId="7" r:id="rId2"/>
     <sheet name="sensitization Ex 5" sheetId="9" r:id="rId3"/>
     <sheet name="learning_genes Ex 6" sheetId="10" r:id="rId4"/>
     <sheet name="habituation" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Emotion_HeartRate Ex 3'!$A$1:$E$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">emotion_heartrate!$A$1:$E$69</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">habituation!$A$1:$D$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'labels_and_flavor Ex 4'!$A$1:$F$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">labels_flavor!$A$1:$F$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'learning_genes Ex 6'!$A$1:$G$13</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -125,12 +125,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,7 +297,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="4" fontId="4" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="4" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,12 +326,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -339,14 +339,6 @@
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -544,6 +536,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor indexed="47"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor indexed="42"/>
         </patternFill>
       </fill>
@@ -579,7 +579,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -604,7 +604,7 @@
           <bgColor indexed="42"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -629,13 +629,18 @@
           <bgColor indexed="42"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2274,16 +2279,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:G13" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:G13" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:G13"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Animal" dataDxfId="7"/>
-    <tableColumn id="2" name="Tissue" dataDxfId="6"/>
-    <tableColumn id="7" name="Trained_Side" dataDxfId="5"/>
-    <tableColumn id="4" name="Egr_Untrained" dataDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="Egr_Trained" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="6" name="CREB_Untrained" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="9" name="CREB_Trained" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="1" name="Animal" dataDxfId="6"/>
+    <tableColumn id="2" name="Tissue" dataDxfId="5"/>
+    <tableColumn id="7" name="Trained_Side" dataDxfId="4"/>
+    <tableColumn id="4" name="Egr_Untrained" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="Egr_Trained" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="CREB_Untrained" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="9" name="CREB_Trained" dataDxfId="0" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2557,21 +2562,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
@@ -2580,7 +2585,7 @@
     <col min="5" max="5" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
@@ -2597,7 +2602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -2614,7 +2619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -2631,7 +2636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -2648,7 +2653,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -2665,7 +2670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -2682,7 +2687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -2699,7 +2704,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -2716,7 +2721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -2733,7 +2738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -2750,7 +2755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -2767,7 +2772,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -2784,7 +2789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -2801,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -2818,7 +2823,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -2835,7 +2840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -2852,7 +2857,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -2869,7 +2874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -2886,7 +2891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -2903,7 +2908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -2920,7 +2925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -2937,7 +2942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -2954,7 +2959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -2971,7 +2976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -2988,7 +2993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -3005,7 +3010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -3022,7 +3027,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -3039,7 +3044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -3056,7 +3061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -3073,7 +3078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -3090,7 +3095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -3107,7 +3112,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -3124,7 +3129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -3141,7 +3146,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -3158,7 +3163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -3175,7 +3180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -3192,7 +3197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -3209,7 +3214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>38</v>
       </c>
@@ -3226,7 +3231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>39</v>
       </c>
@@ -3243,7 +3248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>40</v>
       </c>
@@ -3260,7 +3265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>41</v>
       </c>
@@ -3277,7 +3282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>42</v>
       </c>
@@ -3294,7 +3299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>43</v>
       </c>
@@ -3311,7 +3316,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>44</v>
       </c>
@@ -3328,7 +3333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
         <v>45</v>
       </c>
@@ -3345,7 +3350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
         <v>46</v>
       </c>
@@ -3362,7 +3367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
         <v>48</v>
       </c>
@@ -3379,7 +3384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
         <v>49</v>
       </c>
@@ -3396,7 +3401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>50</v>
       </c>
@@ -3413,7 +3418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
         <v>51</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
         <v>52</v>
       </c>
@@ -3447,7 +3452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>53</v>
       </c>
@@ -3464,7 +3469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
         <v>54</v>
       </c>
@@ -3481,7 +3486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
         <v>55</v>
       </c>
@@ -3498,7 +3503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
         <v>56</v>
       </c>
@@ -3515,7 +3520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
         <v>57</v>
       </c>
@@ -3532,7 +3537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
         <v>58</v>
       </c>
@@ -3549,7 +3554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
         <v>59</v>
       </c>
@@ -3566,7 +3571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
         <v>61</v>
       </c>
@@ -3583,7 +3588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
         <v>62</v>
       </c>
@@ -3600,7 +3605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
         <v>64</v>
       </c>
@@ -3617,7 +3622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
         <v>65</v>
       </c>
@@ -3634,7 +3639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>68</v>
       </c>
@@ -3651,7 +3656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
         <v>69</v>
       </c>
@@ -3668,7 +3673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
         <v>70</v>
       </c>
@@ -3685,7 +3690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
         <v>71</v>
       </c>
@@ -3702,7 +3707,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
         <v>72</v>
       </c>
@@ -3719,7 +3724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
         <v>73</v>
       </c>
@@ -3736,7 +3741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
         <v>74</v>
       </c>
@@ -3764,14 +3769,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -3779,7 +3784,7 @@
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3799,7 +3804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>21</v>
       </c>
@@ -3819,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>22</v>
       </c>
@@ -3839,7 +3844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>23</v>
       </c>
@@ -3859,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>24</v>
       </c>
@@ -3879,7 +3884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>43</v>
       </c>
@@ -3899,7 +3904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3919,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3939,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -3959,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -3979,7 +3984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -3999,7 +4004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -4019,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -4039,7 +4044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -4059,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -4079,7 +4084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -4099,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -4119,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -4139,7 +4144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -4159,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -4179,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -4199,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -4219,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
@@ -4239,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -4259,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
@@ -4279,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
@@ -4299,7 +4304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4319,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4339,7 +4344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4359,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4379,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4399,7 +4404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4419,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4439,7 +4444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4459,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4479,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4499,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4519,7 +4524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4539,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4559,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4579,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4599,7 +4604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4619,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4639,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4659,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4679,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4699,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4719,7 +4724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4739,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4759,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4779,7 +4784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4799,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4830,14 +4835,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -4846,7 +4851,7 @@
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -4866,7 +4871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>801</v>
       </c>
@@ -4886,7 +4891,7 @@
         <v>14.830000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>802</v>
       </c>
@@ -4906,7 +4911,7 @@
         <v>7.93</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>803</v>
       </c>
@@ -4926,7 +4931,7 @@
         <v>15.3125</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>804</v>
       </c>
@@ -4946,7 +4951,7 @@
         <v>11.462499999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>805</v>
       </c>
@@ -4966,7 +4971,7 @@
         <v>8.61</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>806</v>
       </c>
@@ -4986,7 +4991,7 @@
         <v>12.824999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>807</v>
       </c>
@@ -5006,7 +5011,7 @@
         <v>10.475</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>808</v>
       </c>
@@ -5026,7 +5031,7 @@
         <v>10.682500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>838</v>
       </c>
@@ -5046,7 +5051,7 @@
         <v>9.5824999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>839</v>
       </c>
@@ -5066,7 +5071,7 @@
         <v>9.9825000000000017</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>840</v>
       </c>
@@ -5086,7 +5091,7 @@
         <v>11.2475</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>841</v>
       </c>
@@ -5119,20 +5124,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="4" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -5155,7 +5160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>801</v>
       </c>
@@ -5179,7 +5184,7 @@
       </c>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>802</v>
       </c>
@@ -5203,7 +5208,7 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>803</v>
       </c>
@@ -5227,7 +5232,7 @@
       </c>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>804</v>
       </c>
@@ -5251,7 +5256,7 @@
       </c>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>805</v>
       </c>
@@ -5275,7 +5280,7 @@
       </c>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>806</v>
       </c>
@@ -5299,7 +5304,7 @@
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>807</v>
       </c>
@@ -5323,7 +5328,7 @@
       </c>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>808</v>
       </c>
@@ -5347,7 +5352,7 @@
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>838</v>
       </c>
@@ -5371,7 +5376,7 @@
       </c>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>839</v>
       </c>
@@ -5395,7 +5400,7 @@
       </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>840</v>
       </c>
@@ -5419,7 +5424,7 @@
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>841</v>
       </c>
@@ -5460,21 +5465,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -5488,7 +5493,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>532</v>
       </c>
@@ -5502,7 +5507,7 @@
         <v>4.1100000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>536</v>
       </c>
@@ -5516,7 +5521,7 @@
         <v>3.8525</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>533</v>
       </c>
@@ -5530,7 +5535,7 @@
         <v>3.7374999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>531</v>
       </c>
@@ -5544,7 +5549,7 @@
         <v>4.4400000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>538</v>
       </c>
@@ -5558,7 +5563,7 @@
         <v>4.21</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>540</v>
       </c>
@@ -5572,7 +5577,7 @@
         <v>4.1974999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>557</v>
       </c>
@@ -5586,7 +5591,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>548</v>
       </c>
@@ -5600,7 +5605,7 @@
         <v>6.12</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>547</v>
       </c>
@@ -5614,7 +5619,7 @@
         <v>5.6174999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>554</v>
       </c>
@@ -5628,7 +5633,7 @@
         <v>5.9050000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>602</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>4.3375000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>596</v>
       </c>
@@ -5656,7 +5661,7 @@
         <v>4.9524999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>603</v>
       </c>
@@ -5670,7 +5675,7 @@
         <v>4.4375</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>601</v>
       </c>

</xml_diff>